<commit_message>
minor: collect all parent department when parse workbook
</commit_message>
<xml_diff>
--- a/src/bk-user/tests/assets/fake_users.xlsx
+++ b/src/bk-user/tests/assets/fake_users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schneesu/Desktop/bk-user/github/bk-user/src/bk-user/tests/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E685C817-456F-C240-9ED3-9AACBC474EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D4AB99-8489-2C4E-A5DB-5907D397A298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="1120" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44380" yWindow="-14100" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>填写须知：
         1. 每行数据代表一个用户，表头代表用户字段，表格中除组织，直接上级列，其他列均为必填字段。
@@ -276,9 +276,6 @@
     <t>freedom@m.com</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>region-10</t>
   </si>
   <si>
@@ -298,13 +295,37 @@
   </si>
   <si>
     <t>+6313512345675</t>
+  </si>
+  <si>
+    <t>qinshisan</t>
+  </si>
+  <si>
+    <t>秦十三</t>
+  </si>
+  <si>
+    <t>qinshisan@m.com</t>
+  </si>
+  <si>
+    <t>+8613512245671</t>
+  </si>
+  <si>
+    <t>公司/部门C/中心CA/小组CAA</t>
+  </si>
+  <si>
+    <t>solar-system</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -322,6 +343,14 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -341,10 +370,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -360,8 +390,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -674,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,319 +766,355 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1">
         <v>13512345671</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="H7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="I10" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="H11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="1">
+        <v>30</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="D14" s="1" t="s">
         <v>80</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
+        <v>666</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{C7F94303-6416-EE46-A1B0-8189F0532F69}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: modify phone field not required for local data source
</commit_message>
<xml_diff>
--- a/src/bk-user/tests/assets/fake_users.xlsx
+++ b/src/bk-user/tests/assets/fake_users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schneesu/Desktop/bk-user/github/bk-user/src/bk-user/tests/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rolin/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D4AB99-8489-2C4E-A5DB-5907D397A298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2B9CF2-7EE8-2740-AE39-BA1D00F63D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44380" yWindow="-14100" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>填写须知：
         1. 每行数据代表一个用户，表头代表用户字段，表格中除组织，直接上级列，其他列均为必填字段。
@@ -306,9 +306,6 @@
     <t>qinshisan@m.com</t>
   </si>
   <si>
-    <t>+8613512245671</t>
-  </si>
-  <si>
     <t>公司/部门C/中心CA/小组CAA</t>
   </si>
   <si>
@@ -325,11 +322,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -348,8 +345,15 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -386,15 +390,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -410,9 +414,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -450,7 +454,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -556,7 +560,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -698,7 +702,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -709,10 +713,10 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
@@ -723,20 +727,20 @@
     <col min="7" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" ht="409" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="36" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -765,7 +769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -792,7 +796,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -815,13 +819,13 @@
         <v>22</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -850,7 +854,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -879,7 +883,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -902,13 +906,13 @@
         <v>41</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -937,7 +941,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -960,13 +964,13 @@
         <v>54</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -995,7 +999,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>63</v>
       </c>
@@ -1018,13 +1022,13 @@
         <v>67</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
@@ -1053,21 +1057,19 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>17</v>
@@ -1076,13 +1078,13 @@
         <v>30</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>76</v>
       </c>
@@ -1101,16 +1103,17 @@
         <v>666</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C13" r:id="rId1" xr:uid="{C7F94303-6416-EE46-A1B0-8189F0532F69}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
feat: modify phone field not required for local data source (#2163)
</commit_message>
<xml_diff>
--- a/src/bk-user/tests/assets/fake_users.xlsx
+++ b/src/bk-user/tests/assets/fake_users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schneesu/Desktop/bk-user/github/bk-user/src/bk-user/tests/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rolin/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D4AB99-8489-2C4E-A5DB-5907D397A298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2B9CF2-7EE8-2740-AE39-BA1D00F63D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44380" yWindow="-14100" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>填写须知：
         1. 每行数据代表一个用户，表头代表用户字段，表格中除组织，直接上级列，其他列均为必填字段。
@@ -306,9 +306,6 @@
     <t>qinshisan@m.com</t>
   </si>
   <si>
-    <t>+8613512245671</t>
-  </si>
-  <si>
     <t>公司/部门C/中心CA/小组CAA</t>
   </si>
   <si>
@@ -325,11 +322,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -348,8 +345,15 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -386,15 +390,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -410,9 +414,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -450,7 +454,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -556,7 +560,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -698,7 +702,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -709,10 +713,10 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
@@ -723,20 +727,20 @@
     <col min="7" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" ht="409" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="36" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -765,7 +769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -792,7 +796,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -815,13 +819,13 @@
         <v>22</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -850,7 +854,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -879,7 +883,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -902,13 +906,13 @@
         <v>41</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -937,7 +941,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -960,13 +964,13 @@
         <v>54</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -995,7 +999,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>63</v>
       </c>
@@ -1018,13 +1022,13 @@
         <v>67</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
@@ -1053,21 +1057,19 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>17</v>
@@ -1076,13 +1078,13 @@
         <v>30</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>76</v>
       </c>
@@ -1101,16 +1103,17 @@
         <v>666</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C13" r:id="rId1" xr:uid="{C7F94303-6416-EE46-A1B0-8189F0532F69}"/>
   </hyperlinks>

</xml_diff>